<commit_message>
primeira mudança adicionando link
</commit_message>
<xml_diff>
--- a/pesquisa.xlsx
+++ b/pesquisa.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
           <t>Valor</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -456,6 +461,11 @@
           <t>124</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://click1.mercadolivre.com.br/mclics/clicks/external/MLB/count?a=IBWzvroGZTpsmo7HS6ecnn%2BE2DJ7H2Lh2vf6uoZuBZ%2FiDMdGFj5Zr87d3tEtjjTK7iSwv64iLjNmAunPU8v3uHB7vPE8DWRhbFlVEYXZYFKw%2B%2FpkgZsdx%2BaXF5RoU6nqAmqh%2Fas40l43qyETH37Uev8G%2FVkqMoqytJaF0mnT5QL789cAdl6dEjCa7IN8Cl2hjD6nbeToHlds7dRBocfM3y9vjAW3%2BcS4789FRFsqXzhZtNDdbbttm1%2FqOc%2BMspIDsNBDjqkE1aFTs4bOsZztANyfxL926tOnUFNCBlzVrFeb5cVgneIfubF62kZpxUJsi%2FPjzal3vhK5q6Nr%2BfRGrCjoXVKow%2BFKasivD56TUu8ibH%2FunwoqLILqgzWghd%2F%2FILHZVZCwwUneotaLetXf%2FCg1aE12%2FTvq0FxajSWp0wnqcxpz0pHr5qrFPoMWPagxGCFYCTzcoMdXJMe%2B7WzdUCzyHGQlUQoPEaDcuyRLgw%2Fol8OdidFUzVCLddVVsYd57Jd4XGHiRwjh6AtfyNXMJSyDi%2F1xOeTlcYOMdmnGnNlHMSR5hcyg4wGe7vdwMzxK2kcvAl%2FPn%2Fd7jqfYEDJh%2FvoJqkLUgmd%2FBaHcXiwRZwgwJyIe3TkbORrpVtWfEk1uIBYhsqr3w9SvnG4f0Yr8n0f5RJTO28KzMAEukFJ45zKxQccLOAqRwmbQDaaEgu%2FBCp5Px6U5V48sUmakhppgLHdeWRUdgAiDG1zvvP7zE%2FuabbhiJPx45y9VOTgdI0S%2FEhurDD2nk4C975mV4Q%3D%3D&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -468,6 +478,11 @@
           <t>198</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://click1.mercadolivre.com.br/mclics/clicks/external/MLB/count?a=coDdJ7DEks3kW6PblmiJLKya%2F8z%2FDoKC9MNh0w92xnG7X7RMeCVYKDp3tUI3En6NDwqeiKU%2Fi9EWj0evKhC4UUxVKNoTuGkextgianGy5LFe0Jj61o279LX23Hi0wbTyl8DA2PMzKjZXe4RhoMGp9eTigDr6smy9bUHjwAyXBo9VwyY1R9m6z22FeS69fVOI4ND%2BNHPdO%2F1WOPWuBdpoFVaYUfDAupSLGbR7jHRq5X4vUNBGF4newNQBMHq9wPLzax4slmuFL2%2BBkU72zGg16ZksRo%2Bdl23SUoilJOwiYyPfmuWbj1iSAdbfmJfzZS966IUDv6GPHyrFGqivLdX%2BWM%2FhjFzoHGU62eHVQ6djcKbOoEsdEaBDQ0FoeUkXIR69k1g8Bjc5JCWmNAYKrSSW14f99udTkKfB62FizR6xWACO917eeWgho%2Bcfr3ZIJkPYZ03fj7ldGGuS2%2BEv7nukqc66PRyqD7bnT0bzJT7HJ5ZreBoGeOsCIT4Q62DPtbGdpM8SIhdd1Z4nwcK%2Fhh6zOj%2BqOfnyZa860TnlHpFfCWfIB%2B3NfP9hp4L1Cw5Md4I8H9Hccnw70DZmuap9KvPgzgRE8K6xpVVh2a5EqaC5VuAs1TW5acUj0h%2FHSEvPsgFCPhaI9zOrLhIOmdkVJWS4JQfmjfRB%2FWlENE7n6ooy6ngj5EMsMWLA4Va%2BID7uZVecGG9ICd4OFrWI83fxPd%2F%2FWhJ3lF4QOYErTHSCuqmYVHG8g1c1Bt1LhofjYyEF%2FJLtyaVpGvbhcH8mot0W9y5%2FqbY%3D&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -480,124 +495,179 @@
           <t>629</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/controle-xbox-wireless-series-xs-carbon-black/p/MLB16268160#polycard_client=search-nordic&amp;searchVariation=MLB16268160&amp;wid=MLB3998223345&amp;position=4&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Controle joystick sem fio Microsoft Wireless Controller Series X|S Series X e S electric volt</t>
+          <t>Controle Microsoft Xbox Wireless Series X/s Velocity Green Cor Verde</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>430</t>
+          <t>545</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/controle-microsoft-xbox-wireless-series-xs-velocity-green-cor-verde/p/MLB22538792#polycard_client=search-nordic&amp;searchVariation=MLB22538792&amp;wid=MLB3443874399&amp;position=3&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Controle joystick sem fio Microsoft Wireless Controller Series X|S Series X e S deep pink</t>
+          <t>Controle joystick sem fio Microsoft Xbox Elite Series 2 branco</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>499</t>
+          <t>1.080</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/controle-joystick-sem-fio-microsoft-xbox-elite-series-2-branco/p/MLB19627127#polycard_client=search-nordic&amp;searchVariation=MLB19627127&amp;wid=MLB3751953327&amp;position=6&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Base Carregador Controle Xbox Series S X Branco 2 Baterias</t>
+          <t>Controle joystick sem fio Microsoft Wireless Controller Series X|S Series X e S electric volt</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>124</t>
+          <t>430</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/controle-joystick-sem-fio-microsoft-wireless-controller-series-xs-series-x-e-s-electric-volt/p/MLB18030215#polycard_client=search-nordic&amp;searchVariation=MLB18030215&amp;wid=MLB2005787418&amp;position=7&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Capa Silicon Control Xbox Series X S para alças de borracha preta</t>
+          <t>Base Carregador Controle Xbox Series S X Branco 2 Baterias</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>124</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-3361773385-base-carregador-controle-xbox-series-s-x-branco-2-baterias-_JM#polycard_client=search-nordic&amp;position=32&amp;search_layout=grid&amp;type=item&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Base Cooler Xbox Series S Carregador Controle Bateria 800mah</t>
+          <t>Controle joystick sem fio Microsoft Xbox Carbon Black preto</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>198</t>
+          <t>409</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/controle-joystick-sem-fio-microsoft-xbox-carbon-black-preto/p/MLB17483958#polycard_client=search-nordic&amp;searchVariation=MLB17483958&amp;wid=MLB3181675322&amp;position=5&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Analógico Controle Xbox One Series S E X Direcional Original</t>
+          <t>Controle joystick sem fio Microsoft Wireless Controller Series X|S Series X e S deep pink</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>499</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/controle-joystick-sem-fio-microsoft-wireless-controller-series-xs-series-x-e-s-deep-pink/p/MLB22522892#polycard_client=search-nordic&amp;searchVariation=MLB22522892&amp;wid=MLB3584569802&amp;position=13&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Bateria Controle Xbox Séries S X 1200mah Cabo Carregador 3m</t>
+          <t>Controle Joystick Sem Fio Microsoft Xbox X/s Branco</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>428</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/controle-joystick-sem-fio-microsoft-xbox-xs-branco/p/MLB22225047#polycard_client=search-nordic&amp;searchVariation=MLB22225047&amp;wid=MLB5273289302&amp;position=16&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Analógico Controle Para Xbox One Series S E X Direcional </t>
+          <t>Knup GM019 Controle Com Fio Usb Para Computador Rgb Gamepass</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>129</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/knup-gm019-controle-com-fio-usb-para-computador-rgb-gamepass/p/MLB21723314#polycard_client=search-nordic&amp;searchVariation=MLB21723314&amp;wid=MLB4454723210&amp;position=10&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Controle Sem Fio Xbox Sky Cipher Special Edition</t>
+          <t>Para Peças Acessórias De Controle Elite Series 2, Jogo 13 Em</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>499</t>
+          <t>163</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/for-elite-series-2-controller-accessory-parts-13-in-1-game/p/MLB2001851161#polycard_client=search-nordic&amp;searchVariation=MLB2001851161&amp;wid=MLB3866470286&amp;position=9&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Carregador Controle Xbox One Series S X + 2 Baterias 800mah</t>
+          <t>Base Cooler Xbox Series S Carregador Controle Bateria 800mah</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>139</t>
+          <t>198</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-3259868703-base-cooler-xbox-series-s-carregador-controle-bateria-800mah-_JM#polycard_client=search-nordic&amp;position=33&amp;search_layout=grid&amp;type=item&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54</t>
         </is>
       </c>
     </row>
@@ -612,436 +682,621 @@
           <t>414</t>
         </is>
       </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/controle-sem-fio-xbox-wireless-preto-cor-carbon-black/p/MLB23280037#polycard_client=search-nordic&amp;searchVariation=MLB23280037&amp;wid=MLB5181374502&amp;position=17&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Joystick sem fio Microsoft Xbox Y PC Gamepad branco</t>
+          <t>Controle Sem Fio Microsoft Xbox Wireless Series X|s Cor Carbon black</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>469</t>
+          <t>410</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/controle-sem-fio-microsoft-xbox-wireless-series-xs-cor-carbon-black/p/MLB26089834#polycard_client=search-nordic&amp;searchVariation=MLB26089834&amp;wid=MLB3997678171&amp;position=11&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Controle joystick sem fio Microsoft Xbox Wireless Controller Series X|S Series X e S robot white</t>
+          <t>Kontrol Freek Extensor Analógico Grip Control Fps Freek</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>489</t>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-4977470558-kontrol-freek-extensor-analogico-grip-control-fps-freek-_JM?searchVariation=181291740168#polycard_client=search-nordic&amp;searchVariation=181291740168&amp;position=34&amp;search_layout=grid&amp;type=item&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Cabo sem fio Microsoft Control Xbox + USB-c preto</t>
+          <t>Controle Sem Fio Xbox One E Cabo Usb Preto</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>427</t>
+          <t>479</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-4958466016-controle-sem-fio-xbox-one-e-cabo-usb-preto-_JM?searchVariation=181222590974#polycard_client=search-nordic&amp;searchVariation=181222590974&amp;position=35&amp;search_layout=grid&amp;type=item&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Kontrol Freek Extensor Analógico Grip Control Fps Freek</t>
+          <t>Controle joystick sem fio Microsoft Xbox Wireless Controller Series X|S Series X e S robot white</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>414</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/controle-joystick-sem-fio-microsoft-xbox-wireless-controller-series-xs-series-x-e-s-robot-white/p/MLB16268161#polycard_client=search-nordic&amp;searchVariation=MLB16268161&amp;wid=MLB3492668122&amp;position=15&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Controle Sem Fio Microsoft Xbox Wireless Series X|s Cor Carbon black</t>
+          <t>2 Botões Gatilho Lb Rb Para Controle Xbox Séries X S 1914</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>410</t>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-4831376386-2-botoes-gatilho-lb-rb-para-controle-xbox-series-x-s-1914-_JM?searchVariation=183399503185#polycard_client=search-nordic&amp;searchVariation=183399503185&amp;position=36&amp;search_layout=grid&amp;type=item&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Controle Xbox Series Deep Pink</t>
+          <t>Controle Microsoft Xbox One Series X E S</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>489</t>
+          <t>419</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/controle-microsoft-xbox-one-series-x-e-s/p/MLB23097417#polycard_client=search-nordic&amp;searchVariation=MLB23097417&amp;wid=MLB4010266483&amp;position=20&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Controle joystick sem fio Microsoft Wireless Controller Series X|S Series X e S pulse red</t>
+          <t>Botão Gatilho Rb Lb  Para Controle Xbox Series S E X</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>448</t>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-3755920903-boto-gatilho-rb-lb-para-controle-xbox-series-s-e-x-_JM?searchVariation=183324883455#polycard_client=search-nordic&amp;searchVariation=183324883455&amp;position=37&amp;search_layout=grid&amp;type=item&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Controle Sem Fio Microsoft Xbox Series X / S Lunar Shift </t>
+          <t>Joystick Microsoft XBox One v1 Preto sem fio</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>789</t>
+          <t>449</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/joystick-microsoft-xbox-one-v1-preto-sem-fio/p/MLB12384031#polycard_client=search-nordic&amp;searchVariation=MLB12384031&amp;wid=MLB4768575412&amp;position=14&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Botão Gatilho Rb Lb  Para Controle Xbox Series S E X</t>
+          <t>Controle Xbox 360 Sem Fio</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>129</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/controle-xbox-360-sem-fio/p/MLB24648019#polycard_client=search-nordic&amp;searchVariation=MLB24648019&amp;wid=MLB3626412625&amp;position=8&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Controle Sem Fio Xbox  Wireless Preto Cor Carbon Black</t>
+          <t>Carregador Controle Xbox One Series S X + 2 Baterias 800mah</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>415</t>
+          <t>139</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-2712532600-carregador-controle-xbox-one-series-s-x-2-baterias-800mah-_JM?searchVariation=178400028139#polycard_client=search-nordic&amp;searchVariation=178400028139&amp;position=38&amp;search_layout=grid&amp;type=item&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Controle Microsoft Xbox One Series X E S</t>
+          <t>Controle joystick sem fio Microsoft Wireless Controller Series X|S Series X e S pulse red</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>419</t>
+          <t>448</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/controle-joystick-sem-fio-microsoft-wireless-controller-series-xs-series-x-e-s-pulse-red/p/MLB17375584#polycard_client=search-nordic&amp;searchVariation=MLB17375584&amp;wid=MLB5284364390&amp;position=21&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Controle Microsoft Starfield Edition Series X|S, One, Pc</t>
+          <t>Control Freek - Fps Freek Galaxy Xbox Série X/s - Um</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1.597</t>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/control-freek-fps-freek-galaxy-xbox-serie-xs-um/p/MLB20883537#polycard_client=search-nordic&amp;searchVariation=MLB20883537&amp;wid=MLB3798096643&amp;position=24&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Joystick Microsoft XBox One v1 Preto sem fio</t>
+          <t>Analógico Controle Xbox One Series S E X Direcional Original</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>449</t>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-2794264431-analogico-controle-xbox-one-series-s-e-x-direcional-original-_JM#polycard_client=search-nordic&amp;position=39&amp;search_layout=grid&amp;type=item&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2 Botões Do Analógico Para Controle Xbox One Slim Series S</t>
+          <t>Controle Compatível Xbox One Series E Pc C/ Fio Top</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>139</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/controle-compativel-xbox-one-series-e-pc-c-fio-top/p/MLB22366874#polycard_client=search-nordic&amp;searchVariation=MLB22366874&amp;wid=MLB3856360757&amp;position=12&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Controle sem fio Xbox Elite Series 2 Core Red</t>
+          <t>1 Botão Gatilho Rb Lb  Para Controle Xbox Series S E X Preto</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>1.198</t>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-3756445547-1-boto-gatilho-rb-lb-para-controle-xbox-series-s-e-x-preto-_JM?searchVariation=183339333763#polycard_client=search-nordic&amp;searchVariation=183339333763&amp;position=40&amp;search_layout=grid&amp;type=item&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Controle Compatível Xbox One Series E Pc C/ Fio Top</t>
+          <t>Bateria Controle Xbox Séries S X 1200mah Cabo Carregador 3m</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>139</t>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-5111737986-bateria-controle-xbox-series-s-x-1200mah-cabo-carregador-3m-_JM#polycard_client=search-nordic&amp;position=41&amp;search_layout=grid&amp;type=item&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2 Botões Gatilho Lb Rb Para Controle Xbox Séries X S 1914</t>
+          <t>2 Botões Do Analógico Para Controle Xbox One Slim Series S</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-4862989250-2-botoes-do-analogico-para-controle-xbox-one-slim-series-s-_JM?searchVariation=180963648648#polycard_client=search-nordic&amp;searchVariation=180963648648&amp;position=42&amp;search_layout=grid&amp;type=item&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Control Freek - Fps Freek Galaxy Xbox Série X/s - Um</t>
+          <t>Controle sem fio Xbox Elite Series 2 Core Red</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>1.198</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/controle-sem-fio-xbox-elite-series-2-core-red/p/MLB22892331#polycard_client=search-nordic&amp;searchVariation=MLB22892331&amp;wid=MLB3859552111&amp;position=23&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Controle joystick sem fio Microsoft Slim One S branco</t>
+          <t>Joystick sem fio Microsoft Xbox Y PC Gamepad branco</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>429</t>
+          <t>469</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/joystick-sem-fio-microsoft-xbox-y-pc-gamepad-branco/p/MLB37263008#polycard_client=search-nordic&amp;searchVariation=MLB37263008&amp;wid=MLB5281114478&amp;position=19&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Cabo Carregador Para Controle Xbox Series Tipo C 3 Metros</t>
+          <t xml:space="preserve">Analógico Controle Para Xbox One Series S E X Direcional </t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-3445580683-analogico-controle-para-xbox-one-series-s-e-x-direcional-_JM#polycard_client=search-nordic&amp;position=43&amp;search_layout=grid&amp;type=item&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Controle 8bitdo Xbox Ultimate C Com Hall Effect A P/ Cor Cinza Escuro</t>
+          <t xml:space="preserve">Controle Joystick Sem Fio Microsoft Xbox Xbox Series </t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>336</t>
+          <t>425</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-4474529196-controle-joystick-sem-fio-microsoft-xbox-xbox-series-_JM?searchVariation=179921638214#polycard_client=search-nordic&amp;searchVariation=179921638214&amp;position=44&amp;search_layout=grid&amp;type=item&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Controle joystick sem fio Microsoft Xbox Carbon Black preto</t>
+          <t>Controle Sem Fio Xbox Sky Cipher Special Edition</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>409</t>
+          <t>528</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/controle-sem-fio-xbox-sky-cipher-special-edition/p/MLB38804309#polycard_client=search-nordic&amp;searchVariation=MLB38804309&amp;wid=MLB5196273196&amp;position=26&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Carregador Controle Xbox One Series S/x + 2 Baterias 800mah</t>
+          <t>Cabo Carregador Para Controle Xbox Series Tipo C 3 Metros</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>114</t>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-2223135747-cabo-carregador-para-controle-xbox-series-tipo-c-3-metros-_JM#polycard_client=search-nordic&amp;position=45&amp;search_layout=grid&amp;type=item&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1 Botão Gatilho Rb Lb  Para Controle Xbox Series S E X Preto</t>
+          <t>Controle 8bitdo Xbox Ultimate C Com Hall Effect A P/ Cor Cinza Escuro</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>336</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/controle-8bitdo-xbox-ultimate-c-com-hall-effect-a-p-cor-cinza-escuro/p/MLB37637160#polycard_client=search-nordic&amp;searchVariation=MLB37637160&amp;wid=MLB4002623151&amp;position=18&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Controle Sem Fio Xbox Series S X One Pc Original Preto</t>
+          <t>Controle Joystick Sem Fio Microsoft Xbox Shock Blue</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>499</t>
+          <t>519</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/controle-joystick-sem-fio-microsoft-xbox-shock-blue/p/MLB16268159#polycard_client=search-nordic&amp;searchVariation=MLB16268159&amp;wid=MLB3610784199&amp;position=30&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Controle Xbox Series X S Edição Especial Nocturnal Vapor Cor Verde-musgo</t>
+          <t>Capa Silicon Control Xbox Series X S para alças de borracha preta</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>499</t>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/capa-silicon-control-xbox-series-x-s-para-alcas-de-borracha-preta/p/MLB34261805#polycard_client=search-nordic&amp;searchVariation=MLB34261805&amp;wid=MLB4011719819&amp;position=27&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Controle joystick sem fio Microsoft Xbox Wireless Controller Series X|S Series X e S daystrike</t>
+          <t>Controle Joystick Sem Fio Microsoft Xbox Xbox Series X|s Con</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>800</t>
+          <t>454</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-3601791199-controle-joystick-sem-fio-microsoft-xbox-xbox-series-xs-con-_JM?searchVariation=181782924599#polycard_client=search-nordic&amp;searchVariation=181782924599&amp;position=46&amp;search_layout=grid&amp;type=item&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Adaptador Controle De Áudio P/ Headset Xbox One X/s</t>
+          <t>Controle Sem Fio Microsoft Xbox Xt7 Pro Carbon Black</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>189</t>
+          <t>430</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-3986451857-controle-sem-fio-microsoft-xbox-xt7-pro-carbon-black-_JM?searchVariation=182998549084#polycard_client=search-nordic&amp;searchVariation=182998549084&amp;position=47&amp;search_layout=grid&amp;type=item&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Controle Joystick Sem Fio Xbox Series X|s Con</t>
+          <t>Controle Joystick Microsoft Xbox Series X/s White Robot</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>449</t>
+          <t>415</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/controle-joystick-microsoft-xbox-series-xs-white-robot/p/MLB27744165#polycard_client=search-nordic&amp;searchVariation=MLB27744165&amp;wid=MLB5309401862&amp;position=31&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Controlador sem fio Microsoft Xbox rosa choque</t>
+          <t>Controle Sem Fio Xbox Series S X One Pc Original Preto</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>469</t>
+          <t>479</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-3397445599-controle-sem-fio-xbox-series-s-x-one-pc-original-preto-_JM?searchVariation=179421230071#polycard_client=search-nordic&amp;searchVariation=179421230071&amp;position=48&amp;search_layout=grid&amp;type=item&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Suporte De Controle Xbox One, Series S E Series X P/ Celular</t>
+          <t>2 Analógicos 3d Controle + T8 Para Xbox One / One S / Séries</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-2774190133-2-analogicos-3d-controle-t8-para-xbox-one-one-s-series-_JM#polycard_client=search-nordic&amp;position=49&amp;search_layout=grid&amp;type=item&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Controle Joystick Sem Fio Microsoft Xbox Xbox Series </t>
+          <t>Controle Joystick Sem Fio Xbox Series X|s Con</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>425</t>
+          <t>449</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-4474553990-controle-joystick-sem-fio-xbox-series-xs-con-_JM?searchVariation=181872070455#polycard_client=search-nordic&amp;searchVariation=181872070455&amp;position=50&amp;search_layout=grid&amp;type=item&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Controle Sem Fio Microsoft Xbox Elite Série 2 Core Azul</t>
+          <t>Controle Microsoft Starfield Edition Series X|S, One, Pc</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>1.249</t>
+          <t>1.597</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/controle-microsoft-starfield-edition-series-xs-one-pc/p/MLB24045273#polycard_client=search-nordic&amp;searchVariation=MLB24045273&amp;wid=MLB3763294656&amp;position=22&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Controle Joystick Microsoft Xbox Series X/s White Robot</t>
+          <t>Bateria Recarregável Para Controle Xbox One Tampa Traseira C Cor Preto</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>415</t>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/bateria-recarregavel-para-controle-xbox-one-tampa-traseira-c-cor-preto/p/MLB25898760#polycard_client=search-nordic&amp;searchVariation=MLB25898760&amp;wid=MLB3897236370&amp;position=29&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Suporte Gamer para 2 Controles e 1 Headset – Aço Resistente, Apoio para Mesa – Ideal para Videogame – Compatível com PS5, PS4, Xbox Series X|S, Xbox One e Switch</t>
+          <t>Controle joystick sem fio Microsoft Slim One S branco</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>429</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/controle-joystick-sem-fio-microsoft-slim-one-s-branco/p/MLB21685852#polycard_client=search-nordic&amp;searchVariation=MLB21685852&amp;wid=MLB3868783357&amp;position=25&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Controle sem fio Microsoft Xbox Elite wireless controller series 2 preto</t>
+          <t>Controle Joystick Sem Fio Microsoft Xbox Wireless Series X|s Cor Shock Blue</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>1.390</t>
+          <t>519</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>https://www.mercadolivre.com.br/controle-joystick-sem-fio-microsoft-xbox-wireless-series-xs-cor-shock-blue/p/MLB39972584#polycard_client=search-nordic&amp;searchVariation=MLB39972584&amp;wid=MLB5135365484&amp;position=28&amp;search_layout=grid&amp;type=product&amp;tracking_id=42fdeefd-8fa5-49e5-99ce-87042b654a54&amp;sid=search</t>
         </is>
       </c>
     </row>

</xml_diff>